<commit_message>
Update documents of testing
</commit_message>
<xml_diff>
--- a/Reports/Test cases.xlsx
+++ b/Reports/Test cases.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="23040" windowHeight="9335"/>
+    <workbookView windowWidth="18468" windowHeight="9335"/>
   </bookViews>
   <sheets>
     <sheet name="Test Cases" sheetId="1" r:id="rId1"/>
@@ -341,10 +341,10 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
     <numFmt numFmtId="176" formatCode="_-* #\.##0\ &quot;₽&quot;_-;\-* #\.##0\ &quot;₽&quot;_-;_-* \-\ &quot;₽&quot;_-;_-@_-"/>
-    <numFmt numFmtId="177" formatCode="_-* #\.##0.00_-;\-* #\.##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="178" formatCode="_-* #\.##0.00\ &quot;₽&quot;_-;\-* #\.##0.00\ &quot;₽&quot;_-;_-* \-??\ &quot;₽&quot;_-;_-@_-"/>
-    <numFmt numFmtId="179" formatCode="_-* #\.##0_-;\-* #\.##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="180" formatCode="yyyy\-mm\-dd;@"/>
+    <numFmt numFmtId="177" formatCode="_-* #\.##0.00\ &quot;₽&quot;_-;\-* #\.##0.00\ &quot;₽&quot;_-;_-* \-??\ &quot;₽&quot;_-;_-@_-"/>
+    <numFmt numFmtId="178" formatCode="yyyy\-mm\-dd;@"/>
+    <numFmt numFmtId="179" formatCode="_-* #\.##0.00_-;\-* #\.##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="180" formatCode="_-* #\.##0_-;\-* #\.##0_-;_-* &quot;-&quot;_-;_-@_-"/>
   </numFmts>
   <fonts count="26">
     <font>
@@ -397,20 +397,35 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -419,16 +434,45 @@
     </font>
     <font>
       <b/>
-      <sz val="15"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -443,15 +487,32 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color theme="1"/>
+      <sz val="15"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
-      <color theme="0"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -465,45 +526,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
@@ -512,29 +534,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -561,7 +561,91 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -573,49 +657,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -627,55 +681,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -693,19 +705,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -717,25 +723,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -931,30 +931,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top style="thin">
@@ -962,6 +938,21 @@
       </top>
       <bottom style="double">
         <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -985,21 +976,30 @@
       <right/>
       <top/>
       <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
         <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
+      <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
-      <right style="thin">
+      <right style="double">
         <color rgb="FF3F3F3F"/>
       </right>
-      <top style="thin">
+      <top style="double">
         <color rgb="FF3F3F3F"/>
       </top>
-      <bottom style="thin">
+      <bottom style="double">
         <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
@@ -1018,148 +1018,148 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="180" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="9" borderId="20" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="13" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="19" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="19" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="17" borderId="18" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="18" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="19" borderId="20" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="9" borderId="18" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="13" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="21" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="21" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1209,7 +1209,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="180" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="16" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1654,8 +1654,8 @@
   <sheetPr/>
   <dimension ref="A1:K383"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A349" workbookViewId="0">
-      <selection activeCell="M386" sqref="M386"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B371" sqref="B371:C371"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4"/>
@@ -2332,7 +2332,7 @@
         <v>22</v>
       </c>
       <c r="B39" s="25" t="s">
-        <v>3</v>
+        <v>35</v>
       </c>
       <c r="C39" s="25"/>
       <c r="D39" s="26"/>

</xml_diff>